<commit_message>
Added SmartMicro to the analysis
</commit_message>
<xml_diff>
--- a/ROS Message format comparison.xlsx
+++ b/ROS Message format comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Z-BSL-RADARIQ-SharedFiles\R&amp;D\ROS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ROS\radar_msgs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C338D2-6274-4F9A-98E5-68BD874AEB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57DF566D-D1C9-411C-87ED-688E30F58B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9DA62CB-F424-45FC-BAE3-DBC36DDF6E75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9DA62CB-F424-45FC-BAE3-DBC36DDF6E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Repo</t>
   </si>
@@ -437,6 +437,38 @@
   </si>
   <si>
     <t>It is hard to know if the data represents points or detections. Bosh documentation does not help much. https://developer.bosch.com/documents/723993/728200/GPRv1.0+English.pdf/c63aec16-9efe-2520-fd18-bacc54203240</t>
+  </si>
+  <si>
+    <t>https://www.smartmicro.com/fileadmin/media/Downloads/Automotive_Radar/Software/umrr_driver.tar.xz.zip</t>
+  </si>
+  <si>
+    <t>Smart Micro</t>
+  </si>
+  <si>
+    <t>All formats are output inside a PointCloud2 message</t>
+  </si>
+  <si>
+    <t>x
+y
+z
+Object_Number
+Speed
+Heading
+Quality
+Acceleration</t>
+  </si>
+  <si>
+    <t>Range
+Azimuth
+Speed_Radial
+RCS
+Elevation
+Also
+x
+y
+z
+Speed_Radial
+RCS</t>
   </si>
 </sst>
 </file>
@@ -917,13 +949,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8DD287-43BC-4773-A087-281C13E543AC}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,148 +1144,169 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:7" ht="156" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="13" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="24"/>
-    </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="14" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:7" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="14" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
       <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{AAEEA0BA-AF5C-44E4-BB8C-7ABDEA0DA495}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{AD575069-49BF-43AB-B672-F656924E14C4}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{3110B9B7-B533-4F35-95E4-507CDAB26E3F}"/>
-    <hyperlink ref="B17" r:id="rId4" xr:uid="{A6DA06B4-145D-4067-BDE5-F30E62CBF3A4}"/>
-    <hyperlink ref="B16" r:id="rId5" xr:uid="{D91C94F3-A68E-4DDE-AB3F-8D3DCCE0F17F}"/>
-    <hyperlink ref="B15" r:id="rId6" xr:uid="{C011E1C9-99E6-4FBC-BEEA-EC177DCBF4A6}"/>
-    <hyperlink ref="B14" r:id="rId7" xr:uid="{BCF3D4BD-2F37-4639-9CCF-D1D4A1E6A46F}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{7DDC4297-C7ED-481B-AFE4-58D488813FAA}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{37016E56-08FE-4ED5-B0ED-9B1E69764B37}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{280E772F-F7F0-45A5-BEF1-D75AB0200ED1}"/>
+    <hyperlink ref="B18" r:id="rId4" xr:uid="{A6DA06B4-145D-4067-BDE5-F30E62CBF3A4}"/>
+    <hyperlink ref="B17" r:id="rId5" xr:uid="{D91C94F3-A68E-4DDE-AB3F-8D3DCCE0F17F}"/>
+    <hyperlink ref="B16" r:id="rId6" xr:uid="{C011E1C9-99E6-4FBC-BEEA-EC177DCBF4A6}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{BCF3D4BD-2F37-4639-9CCF-D1D4A1E6A46F}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{7DDC4297-C7ED-481B-AFE4-58D488813FAA}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{37016E56-08FE-4ED5-B0ED-9B1E69764B37}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{280E772F-F7F0-45A5-BEF1-D75AB0200ED1}"/>
     <hyperlink ref="B6" r:id="rId11" xr:uid="{C677A4FF-877A-4F82-B2DD-AD1298F8CE08}"/>
     <hyperlink ref="B5" r:id="rId12" xr:uid="{A5A742EA-75FE-4B09-A4E0-D0D580FB5CA6}"/>
     <hyperlink ref="B4" r:id="rId13" xr:uid="{441A665F-086A-4B18-8F28-C3B709771110}"/>
     <hyperlink ref="B8" r:id="rId14" xr:uid="{39CA0A62-A59B-470C-AA66-289A96F8EDF7}"/>
     <hyperlink ref="B9" r:id="rId15" xr:uid="{8FE480B2-AFD4-45F3-B405-2DE4C242A104}"/>
     <hyperlink ref="A9" r:id="rId16" xr:uid="{E3349F72-9A65-4D9D-A913-C741E66B3861}"/>
+    <hyperlink ref="B10" r:id="rId17" xr:uid="{21858337-38AC-4FFB-B8E0-6927FCFD46B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>